<commit_message>
JEAF-3014 Added checks for BeanParam for incompatible types in OpenAPI
</commit_message>
<xml_diff>
--- a/jeaf-message-constants-generator/src/main/resources/Generator-Messages.xlsx
+++ b/jeaf-message-constants-generator/src/main/resources/Generator-Messages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator\jeaf-message-constants-generator\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753827E7-038D-4ACB-A2DF-4BF289B0561D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BBD429-8510-4576-81A7-022B4110EE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
   <si>
     <t>Class-Info</t>
   </si>
@@ -398,6 +398,12 @@
   </si>
   <si>
     <t>LOCAL_FILE_PATH_IN_XMI</t>
+  </si>
+  <si>
+    <t>INCOMAPTIBLE_TYPE_IN_BEAN_PARAM</t>
+  </si>
+  <si>
+    <t>When working with OpenAPI and REST there are some restrictions concerning the data types that can be used in Java. This warning tells you that in a defined "BeanParam" at least one property uses an incompatible type. This will lead to an invalid request / response from an OpenAPI perspective.</t>
   </si>
 </sst>
 </file>
@@ -824,17 +830,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CCAB7F28-ED90-43C0-8A71-42EFC7C2E440}" name="Tabelle15" displayName="Tabelle15" ref="A1:I45" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CCAB7F28-ED90-43C0-8A71-42EFC7C2E440}" name="Tabelle15" displayName="Tabelle15" ref="A1:I45" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{7C654A52-9977-43E8-A408-3E83B7FFBCB6}" name="Message-ID" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{63B44A43-C09D-4F43-8DDA-7B503C755DC2}" name="Name" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{1B9EBE8E-E83D-40C4-BF8C-CEBEDF609E6A}" name="Message-Type" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{2128F7C9-1577-4EF9-89C4-182FBACCF9C2}" name="Trace-Level" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{72BF94A4-5250-4027-9917-1B27919FCD58}" name="Deprecated" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{8346C41A-EDA4-40A7-ACAA-BEF5677FA0BF}" name="Description" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{A46297DB-6DF3-41E6-BC33-98ED34EEEC72}" name="Default-Text" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{79E22CF0-6161-4F16-8B6F-2A8B234B7211}" name="de" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{E6D99DB3-44B4-4830-B1DA-DF181780374F}" name="de_CH" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{7C654A52-9977-43E8-A408-3E83B7FFBCB6}" name="Message-ID" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{63B44A43-C09D-4F43-8DDA-7B503C755DC2}" name="Name" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{1B9EBE8E-E83D-40C4-BF8C-CEBEDF609E6A}" name="Message-Type" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{2128F7C9-1577-4EF9-89C4-182FBACCF9C2}" name="Trace-Level" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{72BF94A4-5250-4027-9917-1B27919FCD58}" name="Deprecated" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{8346C41A-EDA4-40A7-ACAA-BEF5677FA0BF}" name="Description" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{A46297DB-6DF3-41E6-BC33-98ED34EEEC72}" name="Default-Text" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{79E22CF0-6161-4F16-8B6F-2A8B234B7211}" name="de" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{E6D99DB3-44B4-4830-B1DA-DF181780374F}" name="de_CH" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -858,17 +864,17 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0CA772BD-8BBC-4A69-B04B-07ABC6834AB5}" name="Tabelle1" displayName="Tabelle1" ref="A1:I45" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0CA772BD-8BBC-4A69-B04B-07ABC6834AB5}" name="Tabelle1" displayName="Tabelle1" ref="A1:I45" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{99B83EAC-0470-4BBD-BF0F-0B3ED216B509}" name="Message-ID" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{1D0805BB-14A5-46D8-926C-7EF19373398A}" name="Name" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{95D9BE1F-E505-4244-BF73-730083595171}" name="Message-Type" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{3AEE1724-EB57-4317-9B44-58142DC5CE51}" name="Trace-Level" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{BCBCDD70-00BD-4A71-AB02-AEADBAA7CE21}" name="Deprecated" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{8A4D2204-43F3-40F6-BF3B-9C6E5AB6BCD1}" name="Description" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{5D2E8F0C-58F0-4394-8334-DBCC1FF18746}" name="Default-Text" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{ECEC86C7-BC45-4B18-80E4-4C2F755B8A25}" name="de" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{A2C4A677-579B-412F-A217-B5C30A83C750}" name="de_CH" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{99B83EAC-0470-4BBD-BF0F-0B3ED216B509}" name="Message-ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{1D0805BB-14A5-46D8-926C-7EF19373398A}" name="Name" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{95D9BE1F-E505-4244-BF73-730083595171}" name="Message-Type" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{3AEE1724-EB57-4317-9B44-58142DC5CE51}" name="Trace-Level" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{BCBCDD70-00BD-4A71-AB02-AEADBAA7CE21}" name="Deprecated" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{8A4D2204-43F3-40F6-BF3B-9C6E5AB6BCD1}" name="Description" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{5D2E8F0C-58F0-4394-8334-DBCC1FF18746}" name="Default-Text" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{ECEC86C7-BC45-4B18-80E4-4C2F755B8A25}" name="de" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{A2C4A677-579B-412F-A217-B5C30A83C750}" name="de_CH" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1359,7 +1365,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,9 +1462,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>9103</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>